<commit_message>
Web UI module added
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">10.12.17.4</t>
   </si>
   <si>
+    <t xml:space="preserve">cisco</t>
+  </si>
+  <si>
     <t xml:space="preserve">nxos</t>
   </si>
   <si>
@@ -58,7 +61,112 @@
     <t xml:space="preserve">10.12.17.5</t>
   </si>
   <si>
-    <t xml:space="preserve">cisco</t>
+    <t xml:space="preserve">N9K3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N9K20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.12.17.23</t>
   </si>
 </sst>
 </file>
@@ -167,10 +275,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -214,28 +322,394 @@
       <c r="C2" s="1" t="n">
         <v>22</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>